<commit_message>
Modification tableur Gestion de tâches
Ajout et suppression de colonnes
</commit_message>
<xml_diff>
--- a/gestion de projet/Gestion de tâches.xlsx
+++ b/gestion de projet/Gestion de tâches.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25703"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Antoine/GitHub/fr.gl.hopital_de_campagne/gestion de projet/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="TASKS" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">TASKS!$2:$2</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
-  <extLst>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -53,17 +48,17 @@
     <t>DONE</t>
   </si>
   <si>
-    <t>% COMPLETE</t>
-  </si>
-  <si>
     <t>TASK LIST</t>
+  </si>
+  <si>
+    <t>Responsable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="13"/>
       <color theme="4" tint="0.39991454817346722"/>
@@ -82,14 +77,6 @@
       <b/>
       <sz val="13"/>
       <color theme="2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="4" tint="0.39991454817346722"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,11 +129,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -171,12 +158,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -189,10 +170,7 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -203,18 +181,31 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="4" tint="0.39991454817346722"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -288,16 +279,18 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:G6" totalsRowShown="0">
-  <autoFilter ref="B2:G6"/>
+  <autoFilter ref="B2:G6">
+    <filterColumn colId="1"/>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="MY TASKS" dataDxfId="3"/>
+    <tableColumn id="2" name="Responsable" dataDxfId="0"/>
     <tableColumn id="4" name="START DATE"/>
     <tableColumn id="5" name="DUE DATE"/>
-    <tableColumn id="6" name="% COMPLETE" dataDxfId="2"/>
-    <tableColumn id="7" name="DONE" dataDxfId="1">
-      <calculatedColumnFormula>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</calculatedColumnFormula>
+    <tableColumn id="7" name="DONE" dataDxfId="2">
+      <calculatedColumnFormula>--(#REF!&gt;=1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="NOTES" dataDxfId="0"/>
+    <tableColumn id="8" name="NOTES" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Task List" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -503,14 +496,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -518,133 +511,95 @@
   <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="33" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="19.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="2.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="2:7" s="9" customFormat="1" ht="30" customHeight="1">
+      <c r="B1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="2:7" ht="24.95" customHeight="1">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
+      <c r="D2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" ht="24.95" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7">
-        <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="24.95" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="C4" s="5"/>
       <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="7">
-        <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
+      <c r="E4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" ht="24.95" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="9">
-        <v>1</v>
-      </c>
-      <c r="F5" s="10">
-        <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>1</v>
-      </c>
+      <c r="E5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="8"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F6" s="10">
-        <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
+    <row r="6" spans="2:7" ht="24.95" customHeight="1">
+      <c r="F6" s="8"/>
       <c r="G6" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3:E6">
-    <cfRule type="dataBar" priority="6">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="5"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E45B70CA-B6A0-4E88-BB95-1D31570318B9}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="This is not a listed value." error="Please pick a value in the list." sqref="E3:E6">
-      <formula1>"0%,25%,50%,75%,100%"</formula1>
-    </dataValidation>
-  </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.25" footer="0.25"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Maj tableur Gestion de taches
6 tâches créées
</commit_message>
<xml_diff>
--- a/gestion de projet/Gestion de tâches.xlsx
+++ b/gestion de projet/Gestion de tâches.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>MY TASKS</t>
   </si>
@@ -39,12 +39,6 @@
     <t>NOTES</t>
   </si>
   <si>
-    <t>[Task]</t>
-  </si>
-  <si>
-    <t>[Date]</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
@@ -52,6 +46,27 @@
   </si>
   <si>
     <t>Responsable</t>
+  </si>
+  <si>
+    <t>Diagramme E/R</t>
+  </si>
+  <si>
+    <t>Piet</t>
+  </si>
+  <si>
+    <t>1ère version</t>
+  </si>
+  <si>
+    <t>Diagramme cas d'utilisation</t>
+  </si>
+  <si>
+    <t>bouml project</t>
+  </si>
+  <si>
+    <t>Chercher chocolats chaud</t>
+  </si>
+  <si>
+    <t>Action récursive</t>
   </si>
 </sst>
 </file>
@@ -133,7 +148,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -149,9 +164,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -172,6 +184,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -180,6 +201,12 @@
     <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -197,12 +224,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -284,13 +305,13 @@
   </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="MY TASKS" dataDxfId="3"/>
-    <tableColumn id="2" name="Responsable" dataDxfId="0"/>
+    <tableColumn id="2" name="Responsable" dataDxfId="2"/>
     <tableColumn id="4" name="START DATE"/>
     <tableColumn id="5" name="DUE DATE"/>
-    <tableColumn id="7" name="DONE" dataDxfId="2">
+    <tableColumn id="7" name="DONE" dataDxfId="1">
       <calculatedColumnFormula>--(#REF!&gt;=1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="NOTES" dataDxfId="1"/>
+    <tableColumn id="8" name="NOTES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Task List" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -496,7 +517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -511,7 +532,7 @@
   <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="33" customHeight="1"/>
@@ -525,78 +546,90 @@
     <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="9" customFormat="1" ht="30" customHeight="1">
-      <c r="B1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+    <row r="1" spans="2:7" s="8" customFormat="1" ht="30" customHeight="1">
+      <c r="B1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="2:7" ht="24.95" customHeight="1">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="F2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="24.95" customHeight="1">
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="5"/>
+      <c r="B3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5">
+        <v>42087</v>
+      </c>
+      <c r="E3" s="13">
+        <v>42087</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="2:7" ht="24.95" customHeight="1">
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="5"/>
+    <row r="4" spans="2:7" ht="33" customHeight="1">
+      <c r="B4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5">
+        <v>42087</v>
+      </c>
+      <c r="E4" s="13">
+        <v>42092</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="2:7" ht="24.95" customHeight="1">
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="2"/>
+    <row r="5" spans="2:7" ht="36" customHeight="1">
+      <c r="B5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>42087</v>
+      </c>
+      <c r="E5" s="5">
+        <v>42087</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:7" ht="24.95" customHeight="1">
-      <c r="F6" s="8"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="2"/>
     </row>
   </sheetData>

</xml_diff>